<commit_message>
Atualizacao correcao de erros
</commit_message>
<xml_diff>
--- a/senai_spmedgroup_sprint1_bd_manha_Bruno/Modelagens/ModeloFisico.xlsx
+++ b/senai_spmedgroup_sprint1_bd_manha_Bruno/Modelagens/ModeloFisico.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fic\Desktop\MedGroup\Modelagens\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fic\Desktop\MedGroup\senai_spmedgroup_sprint1_bd_manha_Bruno\Modelagens\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FBD59FA-6049-4167-A484-125B5E27E031}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{627DE83C-909D-4B25-831E-2412739A6829}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" xr2:uid="{B419D6EC-B1B6-4118-9289-1BBD46995156}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="97">
   <si>
     <t>Especialidades</t>
   </si>
@@ -310,6 +310,12 @@
   </si>
   <si>
     <t>IdStatusSituacao</t>
+  </si>
+  <si>
+    <t>DataNascimento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Usuarios </t>
   </si>
 </sst>
 </file>
@@ -480,7 +486,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -496,6 +502,20 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="21" fontId="0" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -514,20 +534,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -852,10 +859,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31A9CD8E-6686-4650-8857-3BCBB43A0BC1}">
-  <dimension ref="A1:O29"/>
+  <dimension ref="A1:P29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -875,29 +882,31 @@
     <col min="13" max="13" width="16.88671875" customWidth="1"/>
     <col min="14" max="14" width="13.6640625" customWidth="1"/>
     <col min="15" max="15" width="13.44140625" customWidth="1"/>
+    <col min="16" max="16" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="E1" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="I1" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B1" s="23"/>
+      <c r="E1" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="I1" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -932,8 +941,11 @@
       <c r="O2" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P2" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -968,8 +980,11 @@
       <c r="O3" s="5">
         <v>321</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P3" s="27">
+        <v>36558</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -1004,8 +1019,11 @@
       <c r="O4" s="5">
         <v>132</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P4" s="27">
+        <v>36924</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -1040,8 +1058,11 @@
       <c r="O5" s="5">
         <v>123</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P5" s="27">
+        <v>37289</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -1069,8 +1090,11 @@
       <c r="O6" s="5">
         <v>132</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P6" s="27">
+        <v>37654</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -1098,8 +1122,11 @@
       <c r="O7" s="5">
         <v>123</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P7" s="27">
+        <v>38019</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -1107,28 +1134,28 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="20" t="s">
+      <c r="E9" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="K9" s="21" t="s">
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="K9" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="L9" s="21"/>
-      <c r="M9" s="21"/>
-      <c r="N9" s="21"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -1163,7 +1190,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -1198,7 +1225,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -1233,7 +1260,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -1256,7 +1283,7 @@
         <v>43897.583333333336</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -1267,7 +1294,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -1275,7 +1302,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -1293,17 +1320,17 @@
       <c r="B17" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="16" t="s">
+      <c r="E17" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="K17" s="24" t="s">
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="K17" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="L17" s="24"/>
+      <c r="L17" s="18"/>
       <c r="M17" t="s">
         <v>70</v>
       </c>
@@ -1330,10 +1357,10 @@
       <c r="I18" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="K18" s="23" t="s">
+      <c r="K18" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="L18" s="23" t="s">
+      <c r="L18" s="15" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1359,10 +1386,10 @@
       <c r="I19" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="K19" s="23">
-        <v>1</v>
-      </c>
-      <c r="L19" s="23" t="s">
+      <c r="K19" s="15">
+        <v>1</v>
+      </c>
+      <c r="L19" s="15" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1382,23 +1409,23 @@
       <c r="I20" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="K20" s="23">
-        <v>2</v>
-      </c>
-      <c r="L20" s="23" t="s">
+      <c r="K20" s="15">
+        <v>2</v>
+      </c>
+      <c r="L20" s="15" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="K21" s="23">
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="K21" s="15">
         <v>3</v>
       </c>
-      <c r="L21" s="23" t="s">
+      <c r="L21" s="15" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1448,19 +1475,19 @@
       <c r="C25" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="E25" s="15" t="s">
+      <c r="E25" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="15"/>
-      <c r="J25" s="15"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
       <c r="K25" s="1"/>
-      <c r="L25" s="26" t="s">
+      <c r="L25" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="M25" s="26"/>
+      <c r="M25" s="19"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="12">
@@ -1490,10 +1517,10 @@
       <c r="J26" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="L26" s="25" t="s">
+      <c r="L26" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="M26" s="25"/>
+      <c r="M26" s="16"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="12">
@@ -1523,10 +1550,10 @@
       <c r="J27" s="14">
         <v>0.91666666666666663</v>
       </c>
-      <c r="L27" s="25">
-        <v>1</v>
-      </c>
-      <c r="M27" s="25" t="s">
+      <c r="L27" s="16">
+        <v>1</v>
+      </c>
+      <c r="M27" s="16" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1558,10 +1585,10 @@
       <c r="J28" s="14">
         <v>0.83333333333333337</v>
       </c>
-      <c r="L28" s="25">
-        <v>2</v>
-      </c>
-      <c r="M28" s="25" t="s">
+      <c r="L28" s="16">
+        <v>2</v>
+      </c>
+      <c r="M28" s="16" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1575,25 +1602,25 @@
       <c r="C29" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="L29" s="25">
+      <c r="L29" s="16">
         <v>3</v>
       </c>
-      <c r="M29" s="25" t="s">
+      <c r="M29" s="16" t="s">
         <v>93</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="K9:N9"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="E25:J25"/>
-    <mergeCell ref="E17:I17"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A21:C21"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="E9:I9"/>
+    <mergeCell ref="I1:P1"/>
+    <mergeCell ref="K9:N9"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="E25:J25"/>
+    <mergeCell ref="E17:I17"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="N3" r:id="rId1" xr:uid="{5157202F-56AB-4FF7-A703-98E01E3F228E}"/>

</xml_diff>